<commit_message>
Izjednacavanje data excel fajlova
</commit_message>
<xml_diff>
--- a/results/TestResults.xlsx
+++ b/results/TestResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2287" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2629" uniqueCount="478">
   <si>
     <t>App</t>
   </si>
@@ -1274,6 +1274,180 @@
   </si>
   <si>
     <t>10.12.2025:14:25</t>
+  </si>
+  <si>
+    <t>11.12.2025:11:04</t>
+  </si>
+  <si>
+    <t>11.12.2025:11:08</t>
+  </si>
+  <si>
+    <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1</t>
+  </si>
+  <si>
+    <t>11.12.2025:11:36</t>
+  </si>
+  <si>
+    <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1_11_12_2025_11_36.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:11:38</t>
+  </si>
+  <si>
+    <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1_11_12_2025_11_38.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:11:52</t>
+  </si>
+  <si>
+    <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1_11_12_2025_11_52.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:11:55</t>
+  </si>
+  <si>
+    <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1_11_12_2025_11_55.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:12:03</t>
+  </si>
+  <si>
+    <t>11.12.2025:12:06</t>
+  </si>
+  <si>
+    <t>11.12.2025:12:21</t>
+  </si>
+  <si>
+    <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1_11_12_2025_12_21.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:12:22</t>
+  </si>
+  <si>
+    <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1_11_12_2025_12_22.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:12:24</t>
+  </si>
+  <si>
+    <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1_11_12_2025_12_24.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:12:33</t>
+  </si>
+  <si>
+    <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1_11_12_2025_12_33.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:12:34</t>
+  </si>
+  <si>
+    <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1_11_12_2025_12_34.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:12:35</t>
+  </si>
+  <si>
+    <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1_11_12_2025_12_35.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:12:36</t>
+  </si>
+  <si>
+    <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1_11_12_2025_12_36.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:12:43</t>
+  </si>
+  <si>
+    <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1_11_12_2025_12_43.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:12:55</t>
+  </si>
+  <si>
+    <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1_11_12_2025_12_55.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:12:59</t>
+  </si>
+  <si>
+    <t>11.12.2025:13:00</t>
+  </si>
+  <si>
+    <t>11.12.2025:13:03</t>
+  </si>
+  <si>
+    <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1_11_12_2025_13_03.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:13:07</t>
+  </si>
+  <si>
+    <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1_11_12_2025_13_07.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:19:08</t>
+  </si>
+  <si>
+    <t>Manage_Products-Nickname_Product_Returning_To_Default_Name_[WEB]</t>
+  </si>
+  <si>
+    <t>11.12.2025:20:00</t>
+  </si>
+  <si>
+    <t>Manage_Products-Nickname_Product_Returning_To_Default_Name_[WEB]_11_12_2025_20_00.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:20:01</t>
+  </si>
+  <si>
+    <t>11.12.2025:20:02</t>
+  </si>
+  <si>
+    <t>Manage_Products-Nickname_Product_Returning_To_Default_Name_[WEB]_11_12_2025_20_02.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:20:07</t>
+  </si>
+  <si>
+    <t>Manage_Products-Nickname_Product_Returning_To_Default_Name_[WEB]_11_12_2025_20_07.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:20:11</t>
+  </si>
+  <si>
+    <t>Manage_Products-Nickname_Product_Returning_To_Default_Name_[WEB]_11_12_2025_20_11.jpg</t>
+  </si>
+  <si>
+    <t>11.12.2025:20:12</t>
+  </si>
+  <si>
+    <t>Manage_Products-Nickname_Product_[WEB]</t>
+  </si>
+  <si>
+    <t>11.12.2025:20:29</t>
+  </si>
+  <si>
+    <t>11.12.2025:20:32</t>
+  </si>
+  <si>
+    <t>11.12.2025:20:33</t>
+  </si>
+  <si>
+    <t>11.12.2025:22:03</t>
+  </si>
+  <si>
+    <t>Manage_Products-Nickname_Product_[WEB]_Invalid</t>
+  </si>
+  <si>
+    <t>11.12.2025:22:04</t>
+  </si>
+  <si>
+    <t>11.12.2025:22:06</t>
+  </si>
+  <si>
+    <t>11.12.2025:22:11</t>
   </si>
 </sst>
 </file>
@@ -1929,7 +2103,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2280">
+  <cellXfs count="2622">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4216,6 +4390,348 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5384,7 +5900,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:XFD254"/>
+  <dimension ref="A1:XFD292"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -29149,6 +29665,1108 @@
         <v>53</v>
       </c>
     </row>
+    <row r="255">
+      <c r="B255" t="s" s="2280">
+        <v>393</v>
+      </c>
+      <c r="C255" t="s" s="2281">
+        <v>24</v>
+      </c>
+      <c r="D255" t="s" s="2282">
+        <v>420</v>
+      </c>
+      <c r="E255" t="s" s="2283">
+        <v>13</v>
+      </c>
+      <c r="F255" t="s" s="2284">
+        <v>14</v>
+      </c>
+      <c r="G255" t="s" s="2285">
+        <v>40</v>
+      </c>
+      <c r="H255" t="s" s="2286">
+        <v>14</v>
+      </c>
+      <c r="I255" t="s" s="2287">
+        <v>16</v>
+      </c>
+      <c r="J255" t="s" s="2288">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="B256" t="s" s="2289">
+        <v>393</v>
+      </c>
+      <c r="C256" t="s" s="2290">
+        <v>24</v>
+      </c>
+      <c r="D256" t="s" s="2291">
+        <v>421</v>
+      </c>
+      <c r="E256" t="s" s="2292">
+        <v>13</v>
+      </c>
+      <c r="F256" t="s" s="2293">
+        <v>14</v>
+      </c>
+      <c r="G256" t="s" s="2294">
+        <v>40</v>
+      </c>
+      <c r="H256" t="s" s="2295">
+        <v>14</v>
+      </c>
+      <c r="I256" t="s" s="2296">
+        <v>16</v>
+      </c>
+      <c r="J256" t="s" s="2297">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="B257" t="s" s="2298">
+        <v>422</v>
+      </c>
+      <c r="C257" t="s" s="2299">
+        <v>11</v>
+      </c>
+      <c r="D257" t="s" s="2300">
+        <v>423</v>
+      </c>
+      <c r="E257" t="s" s="2301">
+        <v>13</v>
+      </c>
+      <c r="F257" t="s" s="2302">
+        <v>14</v>
+      </c>
+      <c r="G257" t="s" s="2303">
+        <v>40</v>
+      </c>
+      <c r="H257" t="s" s="2304">
+        <v>14</v>
+      </c>
+      <c r="I257" t="s" s="2305">
+        <v>16</v>
+      </c>
+      <c r="J257" t="s" s="2306">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="B258" t="s" s="2307">
+        <v>422</v>
+      </c>
+      <c r="C258" t="s" s="2308">
+        <v>11</v>
+      </c>
+      <c r="D258" t="s" s="2309">
+        <v>425</v>
+      </c>
+      <c r="E258" t="s" s="2310">
+        <v>13</v>
+      </c>
+      <c r="F258" t="s" s="2311">
+        <v>14</v>
+      </c>
+      <c r="G258" t="s" s="2312">
+        <v>40</v>
+      </c>
+      <c r="H258" t="s" s="2313">
+        <v>14</v>
+      </c>
+      <c r="I258" t="s" s="2314">
+        <v>16</v>
+      </c>
+      <c r="J258" t="s" s="2315">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="B259" t="s" s="2316">
+        <v>422</v>
+      </c>
+      <c r="C259" t="s" s="2317">
+        <v>11</v>
+      </c>
+      <c r="D259" t="s" s="2318">
+        <v>427</v>
+      </c>
+      <c r="E259" t="s" s="2319">
+        <v>13</v>
+      </c>
+      <c r="F259" t="s" s="2320">
+        <v>14</v>
+      </c>
+      <c r="G259" t="s" s="2321">
+        <v>40</v>
+      </c>
+      <c r="H259" t="s" s="2322">
+        <v>14</v>
+      </c>
+      <c r="I259" t="s" s="2323">
+        <v>16</v>
+      </c>
+      <c r="J259" t="s" s="2324">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="B260" t="s" s="2325">
+        <v>422</v>
+      </c>
+      <c r="C260" t="s" s="2326">
+        <v>11</v>
+      </c>
+      <c r="D260" t="s" s="2327">
+        <v>429</v>
+      </c>
+      <c r="E260" t="s" s="2328">
+        <v>13</v>
+      </c>
+      <c r="F260" t="s" s="2329">
+        <v>14</v>
+      </c>
+      <c r="G260" t="s" s="2330">
+        <v>40</v>
+      </c>
+      <c r="H260" t="s" s="2331">
+        <v>14</v>
+      </c>
+      <c r="I260" t="s" s="2332">
+        <v>16</v>
+      </c>
+      <c r="J260" t="s" s="2333">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="B261" t="s" s="2334">
+        <v>422</v>
+      </c>
+      <c r="C261" t="s" s="2335">
+        <v>24</v>
+      </c>
+      <c r="D261" t="s" s="2336">
+        <v>431</v>
+      </c>
+      <c r="E261" t="s" s="2337">
+        <v>13</v>
+      </c>
+      <c r="F261" t="s" s="2338">
+        <v>14</v>
+      </c>
+      <c r="G261" t="s" s="2339">
+        <v>40</v>
+      </c>
+      <c r="H261" t="s" s="2340">
+        <v>14</v>
+      </c>
+      <c r="I261" t="s" s="2341">
+        <v>16</v>
+      </c>
+      <c r="J261" t="s" s="2342">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="B262" t="s" s="2343">
+        <v>422</v>
+      </c>
+      <c r="C262" t="s" s="2344">
+        <v>24</v>
+      </c>
+      <c r="D262" t="s" s="2345">
+        <v>432</v>
+      </c>
+      <c r="E262" t="s" s="2346">
+        <v>13</v>
+      </c>
+      <c r="F262" t="s" s="2347">
+        <v>14</v>
+      </c>
+      <c r="G262" t="s" s="2348">
+        <v>40</v>
+      </c>
+      <c r="H262" t="s" s="2349">
+        <v>14</v>
+      </c>
+      <c r="I262" t="s" s="2350">
+        <v>16</v>
+      </c>
+      <c r="J262" t="s" s="2351">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="B263" t="s" s="2352">
+        <v>422</v>
+      </c>
+      <c r="C263" t="s" s="2353">
+        <v>11</v>
+      </c>
+      <c r="D263" t="s" s="2354">
+        <v>433</v>
+      </c>
+      <c r="E263" t="s" s="2355">
+        <v>13</v>
+      </c>
+      <c r="F263" t="s" s="2356">
+        <v>14</v>
+      </c>
+      <c r="G263" t="s" s="2357">
+        <v>40</v>
+      </c>
+      <c r="H263" t="s" s="2358">
+        <v>14</v>
+      </c>
+      <c r="I263" t="s" s="2359">
+        <v>16</v>
+      </c>
+      <c r="J263" t="s" s="2360">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="B264" t="s" s="2361">
+        <v>422</v>
+      </c>
+      <c r="C264" t="s" s="2362">
+        <v>11</v>
+      </c>
+      <c r="D264" t="s" s="2363">
+        <v>435</v>
+      </c>
+      <c r="E264" t="s" s="2364">
+        <v>13</v>
+      </c>
+      <c r="F264" t="s" s="2365">
+        <v>14</v>
+      </c>
+      <c r="G264" t="s" s="2366">
+        <v>40</v>
+      </c>
+      <c r="H264" t="s" s="2367">
+        <v>14</v>
+      </c>
+      <c r="I264" t="s" s="2368">
+        <v>16</v>
+      </c>
+      <c r="J264" t="s" s="2369">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="B265" t="s" s="2370">
+        <v>422</v>
+      </c>
+      <c r="C265" t="s" s="2371">
+        <v>11</v>
+      </c>
+      <c r="D265" t="s" s="2372">
+        <v>437</v>
+      </c>
+      <c r="E265" t="s" s="2373">
+        <v>13</v>
+      </c>
+      <c r="F265" t="s" s="2374">
+        <v>14</v>
+      </c>
+      <c r="G265" t="s" s="2375">
+        <v>40</v>
+      </c>
+      <c r="H265" t="s" s="2376">
+        <v>14</v>
+      </c>
+      <c r="I265" t="s" s="2377">
+        <v>16</v>
+      </c>
+      <c r="J265" t="s" s="2378">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="B266" t="s" s="2379">
+        <v>422</v>
+      </c>
+      <c r="C266" t="s" s="2380">
+        <v>11</v>
+      </c>
+      <c r="D266" t="s" s="2381">
+        <v>439</v>
+      </c>
+      <c r="E266" t="s" s="2382">
+        <v>13</v>
+      </c>
+      <c r="F266" t="s" s="2383">
+        <v>14</v>
+      </c>
+      <c r="G266" t="s" s="2384">
+        <v>40</v>
+      </c>
+      <c r="H266" t="s" s="2385">
+        <v>14</v>
+      </c>
+      <c r="I266" t="s" s="2386">
+        <v>16</v>
+      </c>
+      <c r="J266" t="s" s="2387">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="B267" t="s" s="2388">
+        <v>422</v>
+      </c>
+      <c r="C267" t="s" s="2389">
+        <v>11</v>
+      </c>
+      <c r="D267" t="s" s="2390">
+        <v>441</v>
+      </c>
+      <c r="E267" t="s" s="2391">
+        <v>13</v>
+      </c>
+      <c r="F267" t="s" s="2392">
+        <v>14</v>
+      </c>
+      <c r="G267" t="s" s="2393">
+        <v>40</v>
+      </c>
+      <c r="H267" t="s" s="2394">
+        <v>14</v>
+      </c>
+      <c r="I267" t="s" s="2395">
+        <v>16</v>
+      </c>
+      <c r="J267" t="s" s="2396">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="B268" t="s" s="2397">
+        <v>422</v>
+      </c>
+      <c r="C268" t="s" s="2398">
+        <v>11</v>
+      </c>
+      <c r="D268" t="s" s="2399">
+        <v>443</v>
+      </c>
+      <c r="E268" t="s" s="2400">
+        <v>13</v>
+      </c>
+      <c r="F268" t="s" s="2401">
+        <v>14</v>
+      </c>
+      <c r="G268" t="s" s="2402">
+        <v>40</v>
+      </c>
+      <c r="H268" t="s" s="2403">
+        <v>14</v>
+      </c>
+      <c r="I268" t="s" s="2404">
+        <v>16</v>
+      </c>
+      <c r="J268" t="s" s="2405">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="B269" t="s" s="2406">
+        <v>422</v>
+      </c>
+      <c r="C269" t="s" s="2407">
+        <v>11</v>
+      </c>
+      <c r="D269" t="s" s="2408">
+        <v>445</v>
+      </c>
+      <c r="E269" t="s" s="2409">
+        <v>13</v>
+      </c>
+      <c r="F269" t="s" s="2410">
+        <v>14</v>
+      </c>
+      <c r="G269" t="s" s="2411">
+        <v>40</v>
+      </c>
+      <c r="H269" t="s" s="2412">
+        <v>14</v>
+      </c>
+      <c r="I269" t="s" s="2413">
+        <v>16</v>
+      </c>
+      <c r="J269" t="s" s="2414">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="B270" t="s" s="2415">
+        <v>422</v>
+      </c>
+      <c r="C270" t="s" s="2416">
+        <v>11</v>
+      </c>
+      <c r="D270" t="s" s="2417">
+        <v>447</v>
+      </c>
+      <c r="E270" t="s" s="2418">
+        <v>13</v>
+      </c>
+      <c r="F270" t="s" s="2419">
+        <v>14</v>
+      </c>
+      <c r="G270" t="s" s="2420">
+        <v>40</v>
+      </c>
+      <c r="H270" t="s" s="2421">
+        <v>14</v>
+      </c>
+      <c r="I270" t="s" s="2422">
+        <v>16</v>
+      </c>
+      <c r="J270" t="s" s="2423">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="B271" t="s" s="2424">
+        <v>422</v>
+      </c>
+      <c r="C271" t="s" s="2425">
+        <v>11</v>
+      </c>
+      <c r="D271" t="s" s="2426">
+        <v>449</v>
+      </c>
+      <c r="E271" t="s" s="2427">
+        <v>13</v>
+      </c>
+      <c r="F271" t="s" s="2428">
+        <v>14</v>
+      </c>
+      <c r="G271" t="s" s="2429">
+        <v>40</v>
+      </c>
+      <c r="H271" t="s" s="2430">
+        <v>14</v>
+      </c>
+      <c r="I271" t="s" s="2431">
+        <v>16</v>
+      </c>
+      <c r="J271" t="s" s="2432">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="B272" t="s" s="2433">
+        <v>422</v>
+      </c>
+      <c r="C272" t="s" s="2434">
+        <v>24</v>
+      </c>
+      <c r="D272" t="s" s="2435">
+        <v>451</v>
+      </c>
+      <c r="E272" t="s" s="2436">
+        <v>13</v>
+      </c>
+      <c r="F272" t="s" s="2437">
+        <v>14</v>
+      </c>
+      <c r="G272" t="s" s="2438">
+        <v>40</v>
+      </c>
+      <c r="H272" t="s" s="2439">
+        <v>14</v>
+      </c>
+      <c r="I272" t="s" s="2440">
+        <v>16</v>
+      </c>
+      <c r="J272" t="s" s="2441">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="B273" t="s" s="2442">
+        <v>422</v>
+      </c>
+      <c r="C273" t="s" s="2443">
+        <v>24</v>
+      </c>
+      <c r="D273" t="s" s="2444">
+        <v>452</v>
+      </c>
+      <c r="E273" t="s" s="2445">
+        <v>13</v>
+      </c>
+      <c r="F273" t="s" s="2446">
+        <v>14</v>
+      </c>
+      <c r="G273" t="s" s="2447">
+        <v>40</v>
+      </c>
+      <c r="H273" t="s" s="2448">
+        <v>14</v>
+      </c>
+      <c r="I273" t="s" s="2449">
+        <v>16</v>
+      </c>
+      <c r="J273" t="s" s="2450">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="B274" t="s" s="2451">
+        <v>422</v>
+      </c>
+      <c r="C274" t="s" s="2452">
+        <v>11</v>
+      </c>
+      <c r="D274" t="s" s="2453">
+        <v>453</v>
+      </c>
+      <c r="E274" t="s" s="2454">
+        <v>13</v>
+      </c>
+      <c r="F274" t="s" s="2455">
+        <v>14</v>
+      </c>
+      <c r="G274" t="s" s="2456">
+        <v>40</v>
+      </c>
+      <c r="H274" t="s" s="2457">
+        <v>14</v>
+      </c>
+      <c r="I274" t="s" s="2458">
+        <v>16</v>
+      </c>
+      <c r="J274" t="s" s="2459">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="B275" t="s" s="2460">
+        <v>422</v>
+      </c>
+      <c r="C275" t="s" s="2461">
+        <v>11</v>
+      </c>
+      <c r="D275" t="s" s="2462">
+        <v>455</v>
+      </c>
+      <c r="E275" t="s" s="2463">
+        <v>13</v>
+      </c>
+      <c r="F275" t="s" s="2464">
+        <v>14</v>
+      </c>
+      <c r="G275" t="s" s="2465">
+        <v>40</v>
+      </c>
+      <c r="H275" t="s" s="2466">
+        <v>14</v>
+      </c>
+      <c r="I275" t="s" s="2467">
+        <v>16</v>
+      </c>
+      <c r="J275" t="s" s="2468">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="B276" t="s" s="2469">
+        <v>422</v>
+      </c>
+      <c r="C276" t="s" s="2470">
+        <v>24</v>
+      </c>
+      <c r="D276" t="s" s="2471">
+        <v>455</v>
+      </c>
+      <c r="E276" t="s" s="2472">
+        <v>13</v>
+      </c>
+      <c r="F276" t="s" s="2473">
+        <v>14</v>
+      </c>
+      <c r="G276" t="s" s="2474">
+        <v>40</v>
+      </c>
+      <c r="H276" t="s" s="2475">
+        <v>14</v>
+      </c>
+      <c r="I276" t="s" s="2476">
+        <v>16</v>
+      </c>
+      <c r="J276" t="s" s="2477">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="B277" t="s" s="2478">
+        <v>422</v>
+      </c>
+      <c r="C277" t="s" s="2479">
+        <v>24</v>
+      </c>
+      <c r="D277" t="s" s="2480">
+        <v>455</v>
+      </c>
+      <c r="E277" t="s" s="2481">
+        <v>13</v>
+      </c>
+      <c r="F277" t="s" s="2482">
+        <v>14</v>
+      </c>
+      <c r="G277" t="s" s="2483">
+        <v>40</v>
+      </c>
+      <c r="H277" t="s" s="2484">
+        <v>14</v>
+      </c>
+      <c r="I277" t="s" s="2485">
+        <v>16</v>
+      </c>
+      <c r="J277" t="s" s="2486">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="B278" t="s" s="2487">
+        <v>422</v>
+      </c>
+      <c r="C278" t="s" s="2488">
+        <v>24</v>
+      </c>
+      <c r="D278" t="s" s="2489">
+        <v>457</v>
+      </c>
+      <c r="E278" t="s" s="2490">
+        <v>13</v>
+      </c>
+      <c r="F278" t="s" s="2491">
+        <v>14</v>
+      </c>
+      <c r="G278" t="s" s="2492">
+        <v>40</v>
+      </c>
+      <c r="H278" t="s" s="2493">
+        <v>14</v>
+      </c>
+      <c r="I278" t="s" s="2494">
+        <v>16</v>
+      </c>
+      <c r="J278" t="s" s="2495">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="B279" t="s" s="2496">
+        <v>458</v>
+      </c>
+      <c r="C279" t="s" s="2497">
+        <v>11</v>
+      </c>
+      <c r="D279" t="s" s="2498">
+        <v>459</v>
+      </c>
+      <c r="E279" t="s" s="2499">
+        <v>13</v>
+      </c>
+      <c r="F279" t="s" s="2500">
+        <v>14</v>
+      </c>
+      <c r="G279" t="s" s="2501">
+        <v>40</v>
+      </c>
+      <c r="H279" t="s" s="2502">
+        <v>14</v>
+      </c>
+      <c r="I279" t="s" s="2503">
+        <v>16</v>
+      </c>
+      <c r="J279" t="s" s="2504">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="B280" t="s" s="2505">
+        <v>458</v>
+      </c>
+      <c r="C280" t="s" s="2506">
+        <v>11</v>
+      </c>
+      <c r="D280" t="s" s="2507">
+        <v>461</v>
+      </c>
+      <c r="E280" t="s" s="2508">
+        <v>13</v>
+      </c>
+      <c r="F280" t="s" s="2509">
+        <v>14</v>
+      </c>
+      <c r="G280" t="s" s="2510">
+        <v>40</v>
+      </c>
+      <c r="H280" t="s" s="2511">
+        <v>14</v>
+      </c>
+      <c r="I280" t="s" s="2512">
+        <v>16</v>
+      </c>
+      <c r="J280" t="s" s="2513">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="B281" t="s" s="2514">
+        <v>458</v>
+      </c>
+      <c r="C281" t="s" s="2515">
+        <v>11</v>
+      </c>
+      <c r="D281" t="s" s="2516">
+        <v>462</v>
+      </c>
+      <c r="E281" t="s" s="2517">
+        <v>13</v>
+      </c>
+      <c r="F281" t="s" s="2518">
+        <v>14</v>
+      </c>
+      <c r="G281" t="s" s="2519">
+        <v>40</v>
+      </c>
+      <c r="H281" t="s" s="2520">
+        <v>14</v>
+      </c>
+      <c r="I281" t="s" s="2521">
+        <v>16</v>
+      </c>
+      <c r="J281" t="s" s="2522">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="B282" t="s" s="2523">
+        <v>458</v>
+      </c>
+      <c r="C282" t="s" s="2524">
+        <v>11</v>
+      </c>
+      <c r="D282" t="s" s="2525">
+        <v>464</v>
+      </c>
+      <c r="E282" t="s" s="2526">
+        <v>13</v>
+      </c>
+      <c r="F282" t="s" s="2527">
+        <v>14</v>
+      </c>
+      <c r="G282" t="s" s="2528">
+        <v>40</v>
+      </c>
+      <c r="H282" t="s" s="2529">
+        <v>14</v>
+      </c>
+      <c r="I282" t="s" s="2530">
+        <v>16</v>
+      </c>
+      <c r="J282" t="s" s="2531">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="B283" t="s" s="2532">
+        <v>458</v>
+      </c>
+      <c r="C283" t="s" s="2533">
+        <v>11</v>
+      </c>
+      <c r="D283" t="s" s="2534">
+        <v>466</v>
+      </c>
+      <c r="E283" t="s" s="2535">
+        <v>13</v>
+      </c>
+      <c r="F283" t="s" s="2536">
+        <v>14</v>
+      </c>
+      <c r="G283" t="s" s="2537">
+        <v>40</v>
+      </c>
+      <c r="H283" t="s" s="2538">
+        <v>14</v>
+      </c>
+      <c r="I283" t="s" s="2539">
+        <v>16</v>
+      </c>
+      <c r="J283" t="s" s="2540">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="B284" t="s" s="2541">
+        <v>458</v>
+      </c>
+      <c r="C284" t="s" s="2542">
+        <v>11</v>
+      </c>
+      <c r="D284" t="s" s="2543">
+        <v>466</v>
+      </c>
+      <c r="E284" t="s" s="2544">
+        <v>13</v>
+      </c>
+      <c r="F284" t="s" s="2545">
+        <v>14</v>
+      </c>
+      <c r="G284" t="s" s="2546">
+        <v>40</v>
+      </c>
+      <c r="H284" t="s" s="2547">
+        <v>14</v>
+      </c>
+      <c r="I284" t="s" s="2548">
+        <v>16</v>
+      </c>
+      <c r="J284" t="s" s="2549">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="B285" t="s" s="2550">
+        <v>458</v>
+      </c>
+      <c r="C285" t="s" s="2551">
+        <v>24</v>
+      </c>
+      <c r="D285" t="s" s="2552">
+        <v>468</v>
+      </c>
+      <c r="E285" t="s" s="2553">
+        <v>13</v>
+      </c>
+      <c r="F285" t="s" s="2554">
+        <v>14</v>
+      </c>
+      <c r="G285" t="s" s="2555">
+        <v>40</v>
+      </c>
+      <c r="H285" t="s" s="2556">
+        <v>14</v>
+      </c>
+      <c r="I285" t="s" s="2557">
+        <v>16</v>
+      </c>
+      <c r="J285" t="s" s="2558">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="B286" t="s" s="2559">
+        <v>469</v>
+      </c>
+      <c r="C286" t="s" s="2560">
+        <v>24</v>
+      </c>
+      <c r="D286" t="s" s="2561">
+        <v>470</v>
+      </c>
+      <c r="E286" t="s" s="2562">
+        <v>13</v>
+      </c>
+      <c r="F286" t="s" s="2563">
+        <v>14</v>
+      </c>
+      <c r="G286" t="s" s="2564">
+        <v>40</v>
+      </c>
+      <c r="H286" t="s" s="2565">
+        <v>14</v>
+      </c>
+      <c r="I286" t="s" s="2566">
+        <v>16</v>
+      </c>
+      <c r="J286" t="s" s="2567">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="B287" t="s" s="2568">
+        <v>469</v>
+      </c>
+      <c r="C287" t="s" s="2569">
+        <v>24</v>
+      </c>
+      <c r="D287" t="s" s="2570">
+        <v>471</v>
+      </c>
+      <c r="E287" t="s" s="2571">
+        <v>13</v>
+      </c>
+      <c r="F287" t="s" s="2572">
+        <v>14</v>
+      </c>
+      <c r="G287" t="s" s="2573">
+        <v>40</v>
+      </c>
+      <c r="H287" t="s" s="2574">
+        <v>14</v>
+      </c>
+      <c r="I287" t="s" s="2575">
+        <v>16</v>
+      </c>
+      <c r="J287" t="s" s="2576">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="B288" t="s" s="2577">
+        <v>389</v>
+      </c>
+      <c r="C288" t="s" s="2578">
+        <v>24</v>
+      </c>
+      <c r="D288" t="s" s="2579">
+        <v>472</v>
+      </c>
+      <c r="E288" t="s" s="2580">
+        <v>13</v>
+      </c>
+      <c r="F288" t="s" s="2581">
+        <v>14</v>
+      </c>
+      <c r="G288" t="s" s="2582">
+        <v>40</v>
+      </c>
+      <c r="H288" t="s" s="2583">
+        <v>14</v>
+      </c>
+      <c r="I288" t="s" s="2584">
+        <v>16</v>
+      </c>
+      <c r="J288" t="s" s="2585">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="B289" t="s" s="2586">
+        <v>469</v>
+      </c>
+      <c r="C289" t="s" s="2587">
+        <v>24</v>
+      </c>
+      <c r="D289" t="s" s="2588">
+        <v>473</v>
+      </c>
+      <c r="E289" t="s" s="2589">
+        <v>13</v>
+      </c>
+      <c r="F289" t="s" s="2590">
+        <v>14</v>
+      </c>
+      <c r="G289" t="s" s="2591">
+        <v>40</v>
+      </c>
+      <c r="H289" t="s" s="2592">
+        <v>14</v>
+      </c>
+      <c r="I289" t="s" s="2593">
+        <v>16</v>
+      </c>
+      <c r="J289" t="s" s="2594">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="B290" t="s" s="2595">
+        <v>474</v>
+      </c>
+      <c r="C290" t="s" s="2596">
+        <v>24</v>
+      </c>
+      <c r="D290" t="s" s="2597">
+        <v>475</v>
+      </c>
+      <c r="E290" t="s" s="2598">
+        <v>13</v>
+      </c>
+      <c r="F290" t="s" s="2599">
+        <v>14</v>
+      </c>
+      <c r="G290" t="s" s="2600">
+        <v>40</v>
+      </c>
+      <c r="H290" t="s" s="2601">
+        <v>14</v>
+      </c>
+      <c r="I290" t="s" s="2602">
+        <v>16</v>
+      </c>
+      <c r="J290" t="s" s="2603">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="B291" t="s" s="2604">
+        <v>268</v>
+      </c>
+      <c r="C291" t="s" s="2605">
+        <v>24</v>
+      </c>
+      <c r="D291" t="s" s="2606">
+        <v>476</v>
+      </c>
+      <c r="E291" t="s" s="2607">
+        <v>13</v>
+      </c>
+      <c r="F291" t="s" s="2608">
+        <v>14</v>
+      </c>
+      <c r="G291" t="s" s="2609">
+        <v>40</v>
+      </c>
+      <c r="H291" t="s" s="2610">
+        <v>14</v>
+      </c>
+      <c r="I291" t="s" s="2611">
+        <v>16</v>
+      </c>
+      <c r="J291" t="s" s="2612">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="B292" t="s" s="2613">
+        <v>268</v>
+      </c>
+      <c r="C292" t="s" s="2614">
+        <v>24</v>
+      </c>
+      <c r="D292" t="s" s="2615">
+        <v>477</v>
+      </c>
+      <c r="E292" t="s" s="2616">
+        <v>13</v>
+      </c>
+      <c r="F292" t="s" s="2617">
+        <v>14</v>
+      </c>
+      <c r="G292" t="s" s="2618">
+        <v>40</v>
+      </c>
+      <c r="H292" t="s" s="2619">
+        <v>14</v>
+      </c>
+      <c r="I292" t="s" s="2620">
+        <v>16</v>
+      </c>
+      <c r="J292" t="s" s="2621">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511806" footer="0.511806"/>
   <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>

</xml_diff>